<commit_message>
adding some parts of the questions and choices
</commit_message>
<xml_diff>
--- a/smart_city_survey.xlsx
+++ b/smart_city_survey.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,71 @@
           <t>سوال 3</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 4</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 5</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 6</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 7</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 8</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 9</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 10</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 11</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 12</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 13</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 14</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 15</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>سوال 16</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -458,6 +523,19 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -467,6 +545,19 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -476,6 +567,19 @@
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -485,6 +589,19 @@
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -494,6 +611,19 @@
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -503,6 +633,19 @@
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -516,6 +659,19 @@
           <t>Option 4</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -529,6 +685,19 @@
           <t>Option 3</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -540,6 +709,253 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>Option 4</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Option 2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Option 4</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Option 3</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Option 1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Option 3</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Option 4</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Option 3</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Option 2</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Option 1</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Option 2</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Option 4</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Option 3</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Option 2</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Option 1</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Option 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3-</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>1-</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>3-</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>1-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>3-</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>6-</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>1-</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>6-</t>
         </is>
       </c>
     </row>

</xml_diff>